<commit_message>
Add document metadata verification
</commit_message>
<xml_diff>
--- a/data/docs/Anexo-4.xlsx
+++ b/data/docs/Anexo-4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marta\Desktop\NUEVO PROGRAMA PNCBN\Evaluacion y seleccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\manoly\MatCom\pncti\data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABCF188-60AA-4D2B-9FA6-6F0ECB88F2A6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F53FDE-0482-4452-81C5-56833937A139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{69B21BFD-30A4-4AAC-962F-F68B9D4FBE39}"/>
   </bookViews>
@@ -23,6 +23,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -458,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -498,8 +508,59 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,63 +588,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -624,7 +628,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -912,7 +916,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -926,7 +930,7 @@
       <selection activeCell="C4" sqref="C4:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
@@ -934,131 +938,137 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:6" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="30">
         <v>67</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="14">
         <f>'Criterio 1'!D22+'Criterio 2'!D19+'Criterio 3'!D20+'Criterio 4'!D16</f>
         <v>371</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
       <c r="F10" s="4">
         <f>F9/4</f>
         <v>92.75</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="39" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="23"/>
+      <c r="C12" s="40"/>
       <c r="D12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="21"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="24"/>
+      <c r="C13" s="41"/>
       <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="31"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C11:C13"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C17:F19"/>
     <mergeCell ref="C9:E9"/>
@@ -1066,12 +1076,6 @@
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C11:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1085,17 +1089,17 @@
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1104,32 +1108,32 @@
       <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="45"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="2:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
@@ -1212,7 +1216,7 @@
       </c>
     </row>
     <row r="20" spans="3:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="4">
@@ -1228,7 +1232,7 @@
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D22" s="4">
@@ -1269,7 +1273,7 @@
       <selection activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
@@ -1277,10 +1281,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1289,32 +1293,32 @@
       <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="45"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1352,7 +1356,7 @@
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="46">
+      <c r="D14" s="44">
         <v>90</v>
       </c>
     </row>
@@ -1360,25 +1364,25 @@
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="45"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="47"/>
+      <c r="D16" s="45"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="47"/>
+      <c r="D17" s="45"/>
     </row>
     <row r="18" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="48"/>
+      <c r="D18" s="46"/>
     </row>
     <row r="19" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="6" t="s">
@@ -1411,7 +1415,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
     <col min="3" max="3" width="48.6640625" customWidth="1"/>
@@ -1419,10 +1423,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1431,32 +1435,32 @@
       <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="45"/>
+      <c r="D9" s="43"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
@@ -1568,7 +1572,7 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="3" max="3" width="51.109375" customWidth="1"/>
@@ -1576,10 +1580,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
@@ -1588,32 +1592,32 @@
       <c r="B4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="42"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="32"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="31"/>
-      <c r="D6" s="33"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="34"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="48"/>
     </row>
     <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">

</xml_diff>